<commit_message>
added header & rebuilt JAR
</commit_message>
<xml_diff>
--- a/newEx.xlsx
+++ b/newEx.xlsx
@@ -12,7 +12,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
   <si>
     <t>Среднее геометрическое</t>
   </si>
@@ -92,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -102,167 +114,181 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="C1" t="n">
-        <v>0.5738592353225479</v>
-      </c>
-      <c r="D1" t="e">
-        <v>#NUM!</v>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.06124765865504738</v>
+        <v>4</v>
+      </c>
+      <c r="B2" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6124446717906635</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1.9246492042510421</v>
+        <v>0.5738592353225479</v>
+      </c>
+      <c r="D2" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5876737941710403</v>
+        <v>0.06124765865504738</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1918417082305378</v>
+        <v>0.6124446717906635</v>
       </c>
       <c r="D3" t="n">
-        <v>2.8623777556892516</v>
+        <v>1.9246492042510421</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>1.9849040773697197</v>
+        <v>0.5876737941710403</v>
       </c>
       <c r="C4" t="n">
-        <v>0.843904518287496</v>
+        <v>0.1918417082305378</v>
       </c>
       <c r="D4" t="n">
-        <v>16.025876639890342</v>
+        <v>2.8623777556892516</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0016100204879278932</v>
+        <v>1.9849040773697197</v>
       </c>
       <c r="C5" t="n">
-        <v>0.04992740272224475</v>
+        <v>0.843904518287496</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.22039843607673437</v>
+        <v>16.025876639890342</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>100.0</v>
+        <v>0.0016100204879278932</v>
       </c>
       <c r="C6" t="n">
-        <v>100.0</v>
+        <v>0.04992740272224475</v>
       </c>
       <c r="D6" t="n">
-        <v>100.0</v>
+        <v>-0.22039843607673437</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>9.595040970967965</v>
+        <v>100.0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3132392476689065</v>
+        <v>100.0</v>
       </c>
       <c r="D7" t="n">
-        <v>1.4872205019839535</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.09145207118098576</v>
+        <v>9.595040970967965</v>
       </c>
       <c r="C8" t="n">
-        <v>0.029391239608936897</v>
+        <v>0.3132392476689065</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.28280175064769086</v>
+        <v>1.4872205019839535</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.10370160291199523</v>
+        <v>-0.09145207118098576</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0930976947491958</v>
+        <v>0.029391239608936897</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6677315914978993</v>
+        <v>-0.28280175064769086</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.3453604883553862</v>
+        <v>0.10370160291199523</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0368032410168108</v>
+        <v>0.0930976947491958</v>
       </c>
       <c r="D10" t="n">
-        <v>8.193206416264637</v>
+        <v>0.6677315914978993</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.997988638933748</v>
+        <v>0.3453604883553862</v>
       </c>
       <c r="C11" t="n">
-        <v>0.133340939360234</v>
+        <v>0.0368032410168108</v>
       </c>
       <c r="D11" t="n">
-        <v>-6.86786604618873</v>
+        <v>8.193206416264637</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B12" t="n">
+        <v>-0.997988638933748</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.133340939360234</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-6.86786604618873</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="n">
         <v>0.9869154384359717</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C13" t="n">
         <v>0.9772454576477301</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D13" t="n">
         <v>9.158010593701611</v>
       </c>
     </row>

</xml_diff>